<commit_message>
Made the code more DRY
And more extensible for future additions
</commit_message>
<xml_diff>
--- a/resources/excel/abs_import_sheet(bas_test).xlsx
+++ b/resources/excel/abs_import_sheet(bas_test).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="-28340" windowWidth="25400" windowHeight="27580" tabRatio="500"/>
+    <workbookView xWindow="14860" yWindow="-28340" windowWidth="25660" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed a bug where looking up ocms id was not done right
</commit_message>
<xml_diff>
--- a/resources/excel/abs_import_sheet(bas_test).xlsx
+++ b/resources/excel/abs_import_sheet(bas_test).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14860" yWindow="-28340" windowWidth="25660" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,20 +77,20 @@
     <t>OB00836</t>
   </si>
   <si>
-    <t>OB0F4K3</t>
-  </si>
-  <si>
     <t>steun</t>
   </si>
   <si>
     <t>c123f4k31d</t>
+  </si>
+  <si>
+    <t>OB00454</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,6 +102,11 @@
       <sz val="14"/>
       <color rgb="FF777777"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,9 +129,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,7 +413,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,13 +503,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>

</xml_diff>